<commit_message>
create veglib.xlsl detailed explanation
</commit_message>
<xml_diff>
--- a/example_data/VegeLib.xlsx
+++ b/example_data/VegeLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xHM\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978C0506-F646-43F1-9DDF-1C1B842F143E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E66B8F-4DB1-4DCF-A9A5-5CAE1B219538}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7350" activeTab="1" xr2:uid="{67301EE8-8712-4249-B216-439A239299BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7350" xr2:uid="{67301EE8-8712-4249-B216-439A239299BA}"/>
   </bookViews>
   <sheets>
     <sheet name="para description" sheetId="1" r:id="rId1"/>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBDB6FC-2329-4307-8267-868252A67AFF}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AD5702-3BF4-4060-91A5-E265261B34C6}">
   <dimension ref="A1:BI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="BI6" sqref="BB6:BI6"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="BE1" sqref="BE1:BE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>